<commit_message>
Finished exporting vue table. Now it's perfect
</commit_message>
<xml_diff>
--- a/storage/sorted_achievements/sortedAchievements.xlsx
+++ b/storage/sorted_achievements/sortedAchievements.xlsx
@@ -15,10 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
-  <si>
-    <t>Место</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>ФИО</t>
   </si>
@@ -26,9 +23,27 @@
     <t>Класс</t>
   </si>
   <si>
+    <t>Категория</t>
+  </si>
+  <si>
+    <t>Тип</t>
+  </si>
+  <si>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>Предмет</t>
+  </si>
+  <si>
     <t>Баллы</t>
   </si>
   <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>11-А</t>
+  </si>
+  <si>
     <t>Проектная и исследовательская деятельность</t>
   </si>
   <si>
@@ -38,18 +53,6 @@
     <t>Proj</t>
   </si>
   <si>
-    <t>школьный</t>
-  </si>
-  <si>
-    <t>призер</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>11-А</t>
-  </si>
-  <si>
     <t>Интеллектуальные соревнования</t>
   </si>
   <si>
@@ -57,12 +60,6 @@
   </si>
   <si>
     <t>Int</t>
-  </si>
-  <si>
-    <t>отборочный</t>
-  </si>
-  <si>
-    <t>победитель</t>
   </si>
   <si>
     <t>Спортивные достижения</t>
@@ -416,7 +413,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,18 +421,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="50.559082" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="24.708252" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="6.998291" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="6.998291" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="3.427734" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="2.285156" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="5.855713" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="4.570313" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="50.559082" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="24.708252" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="10.568848" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="6.998291" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,45 +443,48 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G2">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -495,73 +493,55 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G4">
         <v>10</v>
       </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
       <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed some bugs in exporting vue table
</commit_message>
<xml_diff>
--- a/storage/sorted_achievements/sortedAchievements.xlsx
+++ b/storage/sorted_achievements/sortedAchievements.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>ФИО</t>
   </si>
@@ -35,6 +35,12 @@
     <t>Предмет</t>
   </si>
   <si>
+    <t>Этап</t>
+  </si>
+  <si>
+    <t>Результат</t>
+  </si>
+  <si>
     <t>Баллы</t>
   </si>
   <si>
@@ -44,6 +50,15 @@
     <t>11-А</t>
   </si>
   <si>
+    <t>Проектная и исследовательская деятельность</t>
+  </si>
+  <si>
+    <t>kjk</t>
+  </si>
+  <si>
+    <t>Proj</t>
+  </si>
+  <si>
     <t>Интеллектуальные соревнования</t>
   </si>
   <si>
@@ -62,7 +77,10 @@
     <t>ооо</t>
   </si>
   <si>
-    <t>моя оборона</t>
+    <t>ьььь</t>
+  </si>
+  <si>
+    <t>ииии</t>
   </si>
 </sst>
 </file>
@@ -401,7 +419,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -411,14 +429,16 @@
   <cols>
     <col min="1" max="1" width="4.570313" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="6.998291" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="35.2771" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="50.559082" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="24.708252" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="5.855713" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="6.998291" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,50 +460,126 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3">
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added about page + almost finished export
</commit_message>
<xml_diff>
--- a/storage/sorted_achievements/sortedAchievements.xlsx
+++ b/storage/sorted_achievements/sortedAchievements.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>ФИО</t>
   </si>
@@ -23,7 +23,7 @@
     <t>Класс</t>
   </si>
   <si>
-    <t>Категория</t>
+    <t>Категории</t>
   </si>
   <si>
     <t>Тип</t>
@@ -41,9 +41,6 @@
     <t>Результат</t>
   </si>
   <si>
-    <t>Баллы</t>
-  </si>
-  <si>
     <t>s</t>
   </si>
   <si>
@@ -59,6 +56,12 @@
     <t>Proj</t>
   </si>
   <si>
+    <t>школьный</t>
+  </si>
+  <si>
+    <t>призер</t>
+  </si>
+  <si>
     <t>Интеллектуальные соревнования</t>
   </si>
   <si>
@@ -66,6 +69,12 @@
   </si>
   <si>
     <t>Int</t>
+  </si>
+  <si>
+    <t>отборочный</t>
+  </si>
+  <si>
+    <t>победитель</t>
   </si>
   <si>
     <t>Спортивные достижения</t>
@@ -419,7 +428,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,12 +442,11 @@
     <col min="4" max="4" width="24.708252" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="10.568848" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="9.283447" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="12.854004" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,124 +471,109 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
       </c>
       <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
         <v>13</v>
-      </c>
-      <c r="I2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
       </c>
       <c r="H4" t="s">
         <v>19</v>
       </c>
-      <c r="I4">
-        <v>10</v>
-      </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished exporting vue table to Excel
</commit_message>
<xml_diff>
--- a/storage/sorted_achievements/sortedAchievements.xlsx
+++ b/storage/sorted_achievements/sortedAchievements.xlsx
@@ -15,10 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
-  <si>
-    <t>ФИО</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>Класс</t>
   </si>
@@ -39,9 +36,6 @@
   </si>
   <si>
     <t>Результат</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
   <si>
     <t>11-А</t>
@@ -428,7 +422,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,17 +430,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="4.570313" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="6.998291" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="50.559082" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="24.708252" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="50.559082" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="24.708252" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="10.568848" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="12.854004" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,112 +461,97 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
+      <c r="G4" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="H3" t="s">
+      <c r="C5" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed codestyle in export
</commit_message>
<xml_diff>
--- a/storage/sorted_achievements/sortedAchievements.xlsx
+++ b/storage/sorted_achievements/sortedAchievements.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>Класс</t>
   </si>
@@ -26,12 +26,6 @@
     <t>Тип</t>
   </si>
   <si>
-    <t>Название</t>
-  </si>
-  <si>
-    <t>Предмет</t>
-  </si>
-  <si>
     <t>Этап</t>
   </si>
   <si>
@@ -47,9 +41,6 @@
     <t>kjk</t>
   </si>
   <si>
-    <t>Proj</t>
-  </si>
-  <si>
     <t>школьный</t>
   </si>
   <si>
@@ -62,9 +53,6 @@
     <t>МОШ</t>
   </si>
   <si>
-    <t>Int</t>
-  </si>
-  <si>
     <t>отборочный</t>
   </si>
   <si>
@@ -75,15 +63,6 @@
   </si>
   <si>
     <t>Турнир по баскетболу</t>
-  </si>
-  <si>
-    <t>ооо</t>
-  </si>
-  <si>
-    <t>ьььь</t>
-  </si>
-  <si>
-    <t>ииии</t>
   </si>
 </sst>
 </file>
@@ -422,7 +401,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,13 +412,11 @@
     <col min="1" max="1" width="6.998291" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="50.559082" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="24.708252" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="9.283447" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="12.854004" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,103 +432,73 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
+      <c r="E4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Middlewares correction + error 419 after logout fixed + routing war ordered
</commit_message>
<xml_diff>
--- a/storage/sorted_achievements/sortedAchievements.xlsx
+++ b/storage/sorted_achievements/sortedAchievements.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+  <si>
+    <t>ФИО</t>
+  </si>
   <si>
     <t>Класс</t>
   </si>
@@ -26,43 +29,52 @@
     <t>Тип</t>
   </si>
   <si>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>Предмет</t>
+  </si>
+  <si>
     <t>Этап</t>
   </si>
   <si>
     <t>Результат</t>
   </si>
   <si>
+    <t>s</t>
+  </si>
+  <si>
     <t>11-А</t>
   </si>
   <si>
-    <t>Проектная и исследовательская деятельность</t>
-  </si>
-  <si>
-    <t>kjk</t>
+    <t>Интеллектуальные соревнования</t>
+  </si>
+  <si>
+    <t>МОШ</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>отборочный</t>
+  </si>
+  <si>
+    <t>победитель</t>
+  </si>
+  <si>
+    <t>Спортивные достижения</t>
+  </si>
+  <si>
+    <t>Турнир по баскетболу</t>
+  </si>
+  <si>
+    <t>ооо</t>
+  </si>
+  <si>
+    <t>моя оборона</t>
   </si>
   <si>
     <t>школьный</t>
-  </si>
-  <si>
-    <t>призер</t>
-  </si>
-  <si>
-    <t>Интеллектуальные соревнования</t>
-  </si>
-  <si>
-    <t>МОШ</t>
-  </si>
-  <si>
-    <t>отборочный</t>
-  </si>
-  <si>
-    <t>победитель</t>
-  </si>
-  <si>
-    <t>Спортивные достижения</t>
-  </si>
-  <si>
-    <t>Турнир по баскетболу</t>
   </si>
 </sst>
 </file>
@@ -401,7 +413,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -409,14 +421,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="6.998291" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="50.559082" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="24.708252" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="4.570313" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="35.2771" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="24.708252" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="10.568848" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="13.996582" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="12.854004" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,73 +447,66 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>